<commit_message>
Create the login script and return 400 if the username and password are missing
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/5.authentication-using-access-tokens.xlsx
+++ b/me/4.create-a-restful-api/5.authentication-using-access-tokens.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78B0A85-8FC5-41A1-B679-FFB37095F98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00563FE6-06FD-4CF8-90E4-FC8F0936F5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="introduction" sheetId="1" r:id="rId1"/>
+    <sheet name="login endpoint and 400 status" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>An introduction to authentication using access tokens</t>
   </si>
@@ -95,6 +96,190 @@
   </si>
   <si>
     <t>authentication server nên có thể dễ scale hơn.</t>
+  </si>
+  <si>
+    <t>Create the login script and return 400 if the username and password are missing</t>
+  </si>
+  <si>
+    <t>構成</t>
+  </si>
+  <si>
+    <t>rest-api-php</t>
+  </si>
+  <si>
+    <t>1.api-basics</t>
+  </si>
+  <si>
+    <t>2.http-basics</t>
+  </si>
+  <si>
+    <t>3.rest-and-restful-apis</t>
+  </si>
+  <si>
+    <t>1.access-a-restful-api</t>
+  </si>
+  <si>
+    <t>gists.php</t>
+  </si>
+  <si>
+    <t>index.php</t>
+  </si>
+  <si>
+    <t>2.guzzlehttp</t>
+  </si>
+  <si>
+    <t>3.use-an-sdk</t>
+  </si>
+  <si>
+    <t>4.create-a-restful-api</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>.htaccess</t>
+  </si>
+  <si>
+    <t>bootstrap.php</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>1.create_database.sql</t>
+  </si>
+  <si>
+    <t>2.create_task_table.sql</t>
+  </si>
+  <si>
+    <t>3.insert_task_table.sql</t>
+  </si>
+  <si>
+    <t>4.create_user_table.sql</t>
+  </si>
+  <si>
+    <t>5.link_tasks_to_users.sql</t>
+  </si>
+  <si>
+    <t>src</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>Auth.php</t>
+  </si>
+  <si>
+    <t>Database.php</t>
+  </si>
+  <si>
+    <t>ErrorHandler.php</t>
+  </si>
+  <si>
+    <t>TaskController.php</t>
+  </si>
+  <si>
+    <t>TaskGateway.php</t>
+  </si>
+  <si>
+    <t>UserGateway.php</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>.env</t>
+  </si>
+  <si>
+    <t>composer.json</t>
+  </si>
+  <si>
+    <t>register.php</t>
+  </si>
+  <si>
+    <t>login.php</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\api\login.php</t>
+  </si>
+  <si>
+    <t>&lt;?php</t>
+  </si>
+  <si>
+    <t>declare(strict_types=1);</t>
+  </si>
+  <si>
+    <t>require __DIR__ . "/bootstrap.php";</t>
+  </si>
+  <si>
+    <t>if ($_SERVER["REQUEST_METHOD"] !== "POST") {</t>
+  </si>
+  <si>
+    <t>    http_response_code(405);</t>
+  </si>
+  <si>
+    <t>    header("Allow: POST");</t>
+  </si>
+  <si>
+    <t>    exit;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>$data = (array) json_decode(file_get_contents("php://input"), true);</t>
+  </si>
+  <si>
+    <t>if (</t>
+  </si>
+  <si>
+    <t>    !array_key_exists("username", $data) ||</t>
+  </si>
+  <si>
+    <t>    !array_key_exists("password", $data)</t>
+  </si>
+  <si>
+    <t>) {</t>
+  </si>
+  <si>
+    <t>    http_response_code(400);</t>
+  </si>
+  <si>
+    <t>    echo json_encode(["message" =&gt; "missing login credentials"]);</t>
+  </si>
+  <si>
+    <t>echo json_encode($data);</t>
+  </si>
+  <si>
+    <t>login endpoint sẽ check thông tin user và trả về access token</t>
+  </si>
+  <si>
+    <t>ini_set("display_errors", "On");</t>
+  </si>
+  <si>
+    <t>login endpoint chỉ nhận request từ phương thức POST</t>
+  </si>
+  <si>
+    <t>Check by call api</t>
+  </si>
+  <si>
+    <t>Thông tin login phải có username và password mà mình đã đăng ký</t>
+  </si>
+  <si>
+    <t>Call api /login.php nhưng ko gửi thông tin login -&gt; api trả về 400 status</t>
+  </si>
+  <si>
+    <t>call api /index.php với phương thức GET -&gt; api trả về 405 status</t>
+  </si>
+  <si>
+    <t>Call api /login.php nhưng nhưng gửi thông tin login chỉ có username or password -&gt; api cũng trả về 400 status</t>
+  </si>
+  <si>
+    <t>Call api /login.php có gửi đầy đủ thông tin login username và password -&gt; api trả về 200 status</t>
   </si>
 </sst>
 </file>
@@ -303,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -322,6 +507,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1165,6 +1360,717 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>474990</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>94626</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3BDEE1D-BB01-383F-6BBE-1A4A034E4800}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="14154150"/>
+          <a:ext cx="10076190" cy="4990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA400A36-E31F-E081-4816-B8F140CE6C5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1409700" y="10248900"/>
+          <a:ext cx="47625" cy="6210300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83A4A86E-4D5F-1E8F-6D70-52E5BB28DB3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2171700" y="10067925"/>
+          <a:ext cx="6477000" cy="5895975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>436896</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>28031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794A78D2-EDA4-C413-56A6-7919EFAB9DB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="19869150"/>
+          <a:ext cx="10028571" cy="4352381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{207809DA-D4CC-FC4F-214D-22FF399F2879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2181225" y="12353925"/>
+          <a:ext cx="6810375" cy="10506075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CE5E13B-D447-DFDF-EBC8-C2959F2A8A82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2400300" y="12553950"/>
+          <a:ext cx="495300" cy="11210925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>274981</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>161390</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01DF4127-7E49-9114-2AFA-217D6DD2C9AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="25031700"/>
+          <a:ext cx="9952381" cy="4276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E5F497-1BD8-985F-04D3-032CF229A98E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6515100" y="24917400"/>
+          <a:ext cx="2495550" cy="3086100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DFCEF95-1FE2-89AA-B1EF-F39B83F4F27C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1885950" y="24926925"/>
+          <a:ext cx="2209800" cy="1543050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F6353F2-CA9E-AED6-C2A9-94AE87C5997E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2276475" y="23860125"/>
+          <a:ext cx="38100" cy="5010150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>379749</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>142319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{120586C2-99EF-6023-0A25-D631D2D1B0BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="30175200"/>
+          <a:ext cx="10009524" cy="4447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Arrow Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124879B3-2D6C-0B36-7B09-8E2D958A3A16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5686425" y="30060900"/>
+          <a:ext cx="3762375" cy="3105150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Arrow Connector 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A98DEB44-78B4-DD17-31A0-E430C6AD18C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1666875" y="30051375"/>
+          <a:ext cx="1847850" cy="1590675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{836218CF-109E-CFEF-16DC-1FC3FC54FB04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2066925" y="30051375"/>
+          <a:ext cx="2295525" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1430,7 +2336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:U122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
@@ -4091,4 +4997,3147 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F824FAA5-79FE-4F16-B7CE-8AFE2300CCF6}">
+  <dimension ref="A2:S183"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="O68" sqref="O68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="24"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="24"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="24"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="24"/>
+      <c r="K22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="24"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="24"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="24"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="24"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="24"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="24"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="24"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="24"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="24"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="24"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="24"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="24"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="24"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="24"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="24"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="24"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="6"/>
+      <c r="I51" t="s">
+        <v>47</v>
+      </c>
+      <c r="J51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="6"/>
+      <c r="I60" t="s">
+        <v>47</v>
+      </c>
+      <c r="J60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="6"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="6"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="9"/>
+    </row>
+    <row r="72" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="11"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="11"/>
+      <c r="O73" s="11"/>
+      <c r="P73" s="11"/>
+      <c r="Q73" s="11"/>
+      <c r="R73" s="11"/>
+      <c r="S73" s="12"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="14"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="6"/>
+      <c r="S75" s="14"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="14"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="14"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="14"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="14"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="6"/>
+      <c r="S80" s="14"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="14"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="14"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="14"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84" s="13"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="14"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="14"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" s="13"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="5"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="14"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="14"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" s="13"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+      <c r="O88" s="5"/>
+      <c r="P88" s="5"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="6"/>
+      <c r="S88" s="14"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89" s="13"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="5"/>
+      <c r="N89" s="5"/>
+      <c r="O89" s="5"/>
+      <c r="P89" s="5"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="6"/>
+      <c r="S89" s="14"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" s="13"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="5"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="6"/>
+      <c r="S90" s="14"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" s="13"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="5"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="6"/>
+      <c r="S91" s="14"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="5"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="6"/>
+      <c r="S92" s="14"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="5"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="6"/>
+      <c r="S93" s="14"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94" s="13"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="6"/>
+      <c r="S94" s="14"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95" s="13"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5"/>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="6"/>
+      <c r="S95" s="14"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" s="13"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5"/>
+      <c r="P96" s="5"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="14"/>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A97" s="13"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="6"/>
+      <c r="S97" s="14"/>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A98" s="13"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5"/>
+      <c r="N98" s="5"/>
+      <c r="O98" s="5"/>
+      <c r="P98" s="5"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="6"/>
+      <c r="S98" s="14"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99" s="13"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="5"/>
+      <c r="O99" s="5"/>
+      <c r="P99" s="5"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="6"/>
+      <c r="S99" s="14"/>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A100" s="13"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
+      <c r="O100" s="5"/>
+      <c r="P100" s="5"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="6"/>
+      <c r="S100" s="14"/>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A101" s="13"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="8"/>
+      <c r="O101" s="8"/>
+      <c r="P101" s="8"/>
+      <c r="Q101" s="8"/>
+      <c r="R101" s="9"/>
+      <c r="S101" s="14"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A102" s="13"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
+      <c r="L102" s="5"/>
+      <c r="M102" s="5"/>
+      <c r="N102" s="5"/>
+      <c r="O102" s="5"/>
+      <c r="P102" s="5"/>
+      <c r="Q102" s="5"/>
+      <c r="R102" s="5"/>
+      <c r="S102" s="14"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A103" s="13"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+      <c r="L103" s="5"/>
+      <c r="M103" s="5"/>
+      <c r="N103" s="5"/>
+      <c r="O103" s="5"/>
+      <c r="P103" s="5"/>
+      <c r="Q103" s="5"/>
+      <c r="R103" s="5"/>
+      <c r="S103" s="14"/>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A104" s="13"/>
+      <c r="B104" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="2"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="14"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A105" s="13"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5"/>
+      <c r="M105" s="5"/>
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="5"/>
+      <c r="Q105" s="5"/>
+      <c r="R105" s="6"/>
+      <c r="S105" s="14"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A106" s="13"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="5"/>
+      <c r="M106" s="5"/>
+      <c r="N106" s="5"/>
+      <c r="O106" s="5"/>
+      <c r="P106" s="5"/>
+      <c r="Q106" s="5"/>
+      <c r="R106" s="6"/>
+      <c r="S106" s="14"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A107" s="13"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+      <c r="L107" s="5"/>
+      <c r="M107" s="5"/>
+      <c r="N107" s="5"/>
+      <c r="O107" s="5"/>
+      <c r="P107" s="5"/>
+      <c r="Q107" s="5"/>
+      <c r="R107" s="6"/>
+      <c r="S107" s="14"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A108" s="13"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5"/>
+      <c r="M108" s="5"/>
+      <c r="N108" s="5"/>
+      <c r="O108" s="5"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="6"/>
+      <c r="S108" s="14"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A109" s="13"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
+      <c r="M109" s="5"/>
+      <c r="N109" s="5"/>
+      <c r="O109" s="5"/>
+      <c r="P109" s="5"/>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="6"/>
+      <c r="S109" s="14"/>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A110" s="13"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5"/>
+      <c r="M110" s="5"/>
+      <c r="N110" s="5"/>
+      <c r="O110" s="5"/>
+      <c r="P110" s="5"/>
+      <c r="Q110" s="5"/>
+      <c r="R110" s="6"/>
+      <c r="S110" s="14"/>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A111" s="13"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5"/>
+      <c r="M111" s="5"/>
+      <c r="N111" s="5"/>
+      <c r="O111" s="5"/>
+      <c r="P111" s="5"/>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="6"/>
+      <c r="S111" s="14"/>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A112" s="13"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="5"/>
+      <c r="L112" s="5"/>
+      <c r="M112" s="5"/>
+      <c r="N112" s="5"/>
+      <c r="O112" s="5"/>
+      <c r="P112" s="5"/>
+      <c r="Q112" s="5"/>
+      <c r="R112" s="6"/>
+      <c r="S112" s="14"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" s="13"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+      <c r="I113" s="5"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+      <c r="L113" s="5"/>
+      <c r="M113" s="5"/>
+      <c r="N113" s="5"/>
+      <c r="O113" s="5"/>
+      <c r="P113" s="5"/>
+      <c r="Q113" s="5"/>
+      <c r="R113" s="6"/>
+      <c r="S113" s="14"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A114" s="13"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+      <c r="L114" s="5"/>
+      <c r="M114" s="5"/>
+      <c r="N114" s="5"/>
+      <c r="O114" s="5"/>
+      <c r="P114" s="5"/>
+      <c r="Q114" s="5"/>
+      <c r="R114" s="6"/>
+      <c r="S114" s="14"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" s="13"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+      <c r="M115" s="5"/>
+      <c r="N115" s="5"/>
+      <c r="O115" s="5"/>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="6"/>
+      <c r="S115" s="14"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" s="13"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+      <c r="L116" s="5"/>
+      <c r="M116" s="5"/>
+      <c r="N116" s="5"/>
+      <c r="O116" s="5"/>
+      <c r="P116" s="5"/>
+      <c r="Q116" s="5"/>
+      <c r="R116" s="6"/>
+      <c r="S116" s="14"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" s="13"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="5"/>
+      <c r="L117" s="5"/>
+      <c r="M117" s="5"/>
+      <c r="N117" s="5"/>
+      <c r="O117" s="5"/>
+      <c r="P117" s="5"/>
+      <c r="Q117" s="5"/>
+      <c r="R117" s="6"/>
+      <c r="S117" s="14"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" s="13"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="5"/>
+      <c r="J118" s="5"/>
+      <c r="K118" s="5"/>
+      <c r="L118" s="5"/>
+      <c r="M118" s="5"/>
+      <c r="N118" s="5"/>
+      <c r="O118" s="5"/>
+      <c r="P118" s="5"/>
+      <c r="Q118" s="5"/>
+      <c r="R118" s="6"/>
+      <c r="S118" s="14"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119" s="13"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="5"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="5"/>
+      <c r="L119" s="5"/>
+      <c r="M119" s="5"/>
+      <c r="N119" s="5"/>
+      <c r="O119" s="5"/>
+      <c r="P119" s="5"/>
+      <c r="Q119" s="5"/>
+      <c r="R119" s="6"/>
+      <c r="S119" s="14"/>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120" s="13"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="5"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="5"/>
+      <c r="L120" s="5"/>
+      <c r="M120" s="5"/>
+      <c r="N120" s="5"/>
+      <c r="O120" s="5"/>
+      <c r="P120" s="5"/>
+      <c r="Q120" s="5"/>
+      <c r="R120" s="6"/>
+      <c r="S120" s="14"/>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121" s="13"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="5"/>
+      <c r="J121" s="5"/>
+      <c r="K121" s="5"/>
+      <c r="L121" s="5"/>
+      <c r="M121" s="5"/>
+      <c r="N121" s="5"/>
+      <c r="O121" s="5"/>
+      <c r="P121" s="5"/>
+      <c r="Q121" s="5"/>
+      <c r="R121" s="6"/>
+      <c r="S121" s="14"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122" s="13"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+      <c r="I122" s="5"/>
+      <c r="J122" s="5"/>
+      <c r="K122" s="5"/>
+      <c r="L122" s="5"/>
+      <c r="M122" s="5"/>
+      <c r="N122" s="5"/>
+      <c r="O122" s="5"/>
+      <c r="P122" s="5"/>
+      <c r="Q122" s="5"/>
+      <c r="R122" s="6"/>
+      <c r="S122" s="14"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" s="13"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
+      <c r="H123" s="5"/>
+      <c r="I123" s="5"/>
+      <c r="J123" s="5"/>
+      <c r="K123" s="5"/>
+      <c r="L123" s="5"/>
+      <c r="M123" s="5"/>
+      <c r="N123" s="5"/>
+      <c r="O123" s="5"/>
+      <c r="P123" s="5"/>
+      <c r="Q123" s="5"/>
+      <c r="R123" s="6"/>
+      <c r="S123" s="14"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124" s="13"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="5"/>
+      <c r="I124" s="5"/>
+      <c r="J124" s="5"/>
+      <c r="K124" s="5"/>
+      <c r="L124" s="5"/>
+      <c r="M124" s="5"/>
+      <c r="N124" s="5"/>
+      <c r="O124" s="5"/>
+      <c r="P124" s="5"/>
+      <c r="Q124" s="5"/>
+      <c r="R124" s="6"/>
+      <c r="S124" s="14"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125" s="13"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="5"/>
+      <c r="I125" s="5"/>
+      <c r="J125" s="5"/>
+      <c r="K125" s="5"/>
+      <c r="L125" s="5"/>
+      <c r="M125" s="5"/>
+      <c r="N125" s="5"/>
+      <c r="O125" s="5"/>
+      <c r="P125" s="5"/>
+      <c r="Q125" s="5"/>
+      <c r="R125" s="6"/>
+      <c r="S125" s="14"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126" s="13"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="5"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="5"/>
+      <c r="L126" s="5"/>
+      <c r="M126" s="5"/>
+      <c r="N126" s="5"/>
+      <c r="O126" s="5"/>
+      <c r="P126" s="5"/>
+      <c r="Q126" s="5"/>
+      <c r="R126" s="6"/>
+      <c r="S126" s="14"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" s="13"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="5"/>
+      <c r="I127" s="5"/>
+      <c r="J127" s="5"/>
+      <c r="K127" s="5"/>
+      <c r="L127" s="5"/>
+      <c r="M127" s="5"/>
+      <c r="N127" s="5"/>
+      <c r="O127" s="5"/>
+      <c r="P127" s="5"/>
+      <c r="Q127" s="5"/>
+      <c r="R127" s="6"/>
+      <c r="S127" s="14"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128" s="13"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="8"/>
+      <c r="J128" s="8"/>
+      <c r="K128" s="8"/>
+      <c r="L128" s="8"/>
+      <c r="M128" s="8"/>
+      <c r="N128" s="8"/>
+      <c r="O128" s="8"/>
+      <c r="P128" s="8"/>
+      <c r="Q128" s="8"/>
+      <c r="R128" s="9"/>
+      <c r="S128" s="14"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129" s="13"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
+      <c r="H129" s="5"/>
+      <c r="I129" s="5"/>
+      <c r="J129" s="5"/>
+      <c r="K129" s="5"/>
+      <c r="L129" s="5"/>
+      <c r="M129" s="5"/>
+      <c r="N129" s="5"/>
+      <c r="O129" s="5"/>
+      <c r="P129" s="5"/>
+      <c r="Q129" s="5"/>
+      <c r="R129" s="5"/>
+      <c r="S129" s="14"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" s="13"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="5"/>
+      <c r="I130" s="5"/>
+      <c r="J130" s="5"/>
+      <c r="K130" s="5"/>
+      <c r="L130" s="5"/>
+      <c r="M130" s="5"/>
+      <c r="N130" s="5"/>
+      <c r="O130" s="5"/>
+      <c r="P130" s="5"/>
+      <c r="Q130" s="5"/>
+      <c r="R130" s="5"/>
+      <c r="S130" s="14"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131" s="13"/>
+      <c r="B131" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+      <c r="L131" s="2"/>
+      <c r="M131" s="2"/>
+      <c r="N131" s="2"/>
+      <c r="O131" s="2"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" s="2"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="14"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A132" s="13"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="5"/>
+      <c r="I132" s="5"/>
+      <c r="J132" s="5"/>
+      <c r="K132" s="5"/>
+      <c r="L132" s="5"/>
+      <c r="M132" s="5"/>
+      <c r="N132" s="5"/>
+      <c r="O132" s="5"/>
+      <c r="P132" s="5"/>
+      <c r="Q132" s="5"/>
+      <c r="R132" s="6"/>
+      <c r="S132" s="14"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" s="13"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5"/>
+      <c r="H133" s="5"/>
+      <c r="I133" s="5"/>
+      <c r="J133" s="5"/>
+      <c r="K133" s="5"/>
+      <c r="L133" s="5"/>
+      <c r="M133" s="5"/>
+      <c r="N133" s="5"/>
+      <c r="O133" s="5"/>
+      <c r="P133" s="5"/>
+      <c r="Q133" s="5"/>
+      <c r="R133" s="6"/>
+      <c r="S133" s="14"/>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" s="13"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+      <c r="G134" s="5"/>
+      <c r="H134" s="5"/>
+      <c r="I134" s="5"/>
+      <c r="J134" s="5"/>
+      <c r="K134" s="5"/>
+      <c r="L134" s="5"/>
+      <c r="M134" s="5"/>
+      <c r="N134" s="5"/>
+      <c r="O134" s="5"/>
+      <c r="P134" s="5"/>
+      <c r="Q134" s="5"/>
+      <c r="R134" s="6"/>
+      <c r="S134" s="14"/>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" s="13"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+      <c r="G135" s="5"/>
+      <c r="H135" s="5"/>
+      <c r="I135" s="5"/>
+      <c r="J135" s="5"/>
+      <c r="K135" s="5"/>
+      <c r="L135" s="5"/>
+      <c r="M135" s="5"/>
+      <c r="N135" s="5"/>
+      <c r="O135" s="5"/>
+      <c r="P135" s="5"/>
+      <c r="Q135" s="5"/>
+      <c r="R135" s="6"/>
+      <c r="S135" s="14"/>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" s="13"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="5"/>
+      <c r="I136" s="5"/>
+      <c r="J136" s="5"/>
+      <c r="K136" s="5"/>
+      <c r="L136" s="5"/>
+      <c r="M136" s="5"/>
+      <c r="N136" s="5"/>
+      <c r="O136" s="5"/>
+      <c r="P136" s="5"/>
+      <c r="Q136" s="5"/>
+      <c r="R136" s="6"/>
+      <c r="S136" s="14"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" s="13"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+      <c r="G137" s="5"/>
+      <c r="H137" s="5"/>
+      <c r="I137" s="5"/>
+      <c r="J137" s="5"/>
+      <c r="K137" s="5"/>
+      <c r="L137" s="5"/>
+      <c r="M137" s="5"/>
+      <c r="N137" s="5"/>
+      <c r="O137" s="5"/>
+      <c r="P137" s="5"/>
+      <c r="Q137" s="5"/>
+      <c r="R137" s="6"/>
+      <c r="S137" s="14"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" s="13"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+      <c r="I138" s="5"/>
+      <c r="J138" s="5"/>
+      <c r="K138" s="5"/>
+      <c r="L138" s="5"/>
+      <c r="M138" s="5"/>
+      <c r="N138" s="5"/>
+      <c r="O138" s="5"/>
+      <c r="P138" s="5"/>
+      <c r="Q138" s="5"/>
+      <c r="R138" s="6"/>
+      <c r="S138" s="14"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" s="13"/>
+      <c r="B139" s="4"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="5"/>
+      <c r="I139" s="5"/>
+      <c r="J139" s="5"/>
+      <c r="K139" s="5"/>
+      <c r="L139" s="5"/>
+      <c r="M139" s="5"/>
+      <c r="N139" s="5"/>
+      <c r="O139" s="5"/>
+      <c r="P139" s="5"/>
+      <c r="Q139" s="5"/>
+      <c r="R139" s="6"/>
+      <c r="S139" s="14"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" s="13"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="5"/>
+      <c r="I140" s="5"/>
+      <c r="J140" s="5"/>
+      <c r="K140" s="5"/>
+      <c r="L140" s="5"/>
+      <c r="M140" s="5"/>
+      <c r="N140" s="5"/>
+      <c r="O140" s="5"/>
+      <c r="P140" s="5"/>
+      <c r="Q140" s="5"/>
+      <c r="R140" s="6"/>
+      <c r="S140" s="14"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" s="13"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="5"/>
+      <c r="J141" s="5"/>
+      <c r="K141" s="5"/>
+      <c r="L141" s="5"/>
+      <c r="M141" s="5"/>
+      <c r="N141" s="5"/>
+      <c r="O141" s="5"/>
+      <c r="P141" s="5"/>
+      <c r="Q141" s="5"/>
+      <c r="R141" s="6"/>
+      <c r="S141" s="14"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" s="13"/>
+      <c r="B142" s="4"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="5"/>
+      <c r="J142" s="5"/>
+      <c r="K142" s="5"/>
+      <c r="L142" s="5"/>
+      <c r="M142" s="5"/>
+      <c r="N142" s="5"/>
+      <c r="O142" s="5"/>
+      <c r="P142" s="5"/>
+      <c r="Q142" s="5"/>
+      <c r="R142" s="6"/>
+      <c r="S142" s="14"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" s="13"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5"/>
+      <c r="H143" s="5"/>
+      <c r="I143" s="5"/>
+      <c r="J143" s="5"/>
+      <c r="K143" s="5"/>
+      <c r="L143" s="5"/>
+      <c r="M143" s="5"/>
+      <c r="N143" s="5"/>
+      <c r="O143" s="5"/>
+      <c r="P143" s="5"/>
+      <c r="Q143" s="5"/>
+      <c r="R143" s="6"/>
+      <c r="S143" s="14"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" s="13"/>
+      <c r="B144" s="4"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5"/>
+      <c r="H144" s="5"/>
+      <c r="I144" s="5"/>
+      <c r="J144" s="5"/>
+      <c r="K144" s="5"/>
+      <c r="L144" s="5"/>
+      <c r="M144" s="5"/>
+      <c r="N144" s="5"/>
+      <c r="O144" s="5"/>
+      <c r="P144" s="5"/>
+      <c r="Q144" s="5"/>
+      <c r="R144" s="6"/>
+      <c r="S144" s="14"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" s="13"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+      <c r="I145" s="5"/>
+      <c r="J145" s="5"/>
+      <c r="K145" s="5"/>
+      <c r="L145" s="5"/>
+      <c r="M145" s="5"/>
+      <c r="N145" s="5"/>
+      <c r="O145" s="5"/>
+      <c r="P145" s="5"/>
+      <c r="Q145" s="5"/>
+      <c r="R145" s="6"/>
+      <c r="S145" s="14"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" s="13"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="J146" s="5"/>
+      <c r="K146" s="5"/>
+      <c r="L146" s="5"/>
+      <c r="M146" s="5"/>
+      <c r="N146" s="5"/>
+      <c r="O146" s="5"/>
+      <c r="P146" s="5"/>
+      <c r="Q146" s="5"/>
+      <c r="R146" s="6"/>
+      <c r="S146" s="14"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" s="13"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5"/>
+      <c r="H147" s="5"/>
+      <c r="I147" s="5"/>
+      <c r="J147" s="5"/>
+      <c r="K147" s="5"/>
+      <c r="L147" s="5"/>
+      <c r="M147" s="5"/>
+      <c r="N147" s="5"/>
+      <c r="O147" s="5"/>
+      <c r="P147" s="5"/>
+      <c r="Q147" s="5"/>
+      <c r="R147" s="6"/>
+      <c r="S147" s="14"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" s="13"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+      <c r="G148" s="5"/>
+      <c r="H148" s="5"/>
+      <c r="I148" s="5"/>
+      <c r="J148" s="5"/>
+      <c r="K148" s="5"/>
+      <c r="L148" s="5"/>
+      <c r="M148" s="5"/>
+      <c r="N148" s="5"/>
+      <c r="O148" s="5"/>
+      <c r="P148" s="5"/>
+      <c r="Q148" s="5"/>
+      <c r="R148" s="6"/>
+      <c r="S148" s="14"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A149" s="13"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5"/>
+      <c r="H149" s="5"/>
+      <c r="I149" s="5"/>
+      <c r="J149" s="5"/>
+      <c r="K149" s="5"/>
+      <c r="L149" s="5"/>
+      <c r="M149" s="5"/>
+      <c r="N149" s="5"/>
+      <c r="O149" s="5"/>
+      <c r="P149" s="5"/>
+      <c r="Q149" s="5"/>
+      <c r="R149" s="6"/>
+      <c r="S149" s="14"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A150" s="13"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="5"/>
+      <c r="I150" s="5"/>
+      <c r="J150" s="5"/>
+      <c r="K150" s="5"/>
+      <c r="L150" s="5"/>
+      <c r="M150" s="5"/>
+      <c r="N150" s="5"/>
+      <c r="O150" s="5"/>
+      <c r="P150" s="5"/>
+      <c r="Q150" s="5"/>
+      <c r="R150" s="6"/>
+      <c r="S150" s="14"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A151" s="13"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="5"/>
+      <c r="H151" s="5"/>
+      <c r="I151" s="5"/>
+      <c r="J151" s="5"/>
+      <c r="K151" s="5"/>
+      <c r="L151" s="5"/>
+      <c r="M151" s="5"/>
+      <c r="N151" s="5"/>
+      <c r="O151" s="5"/>
+      <c r="P151" s="5"/>
+      <c r="Q151" s="5"/>
+      <c r="R151" s="6"/>
+      <c r="S151" s="14"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A152" s="13"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="5"/>
+      <c r="I152" s="5"/>
+      <c r="J152" s="5"/>
+      <c r="K152" s="5"/>
+      <c r="L152" s="5"/>
+      <c r="M152" s="5"/>
+      <c r="N152" s="5"/>
+      <c r="O152" s="5"/>
+      <c r="P152" s="5"/>
+      <c r="Q152" s="5"/>
+      <c r="R152" s="6"/>
+      <c r="S152" s="14"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A153" s="13"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+      <c r="G153" s="5"/>
+      <c r="H153" s="5"/>
+      <c r="I153" s="5"/>
+      <c r="J153" s="5"/>
+      <c r="K153" s="5"/>
+      <c r="L153" s="5"/>
+      <c r="M153" s="5"/>
+      <c r="N153" s="5"/>
+      <c r="O153" s="5"/>
+      <c r="P153" s="5"/>
+      <c r="Q153" s="5"/>
+      <c r="R153" s="6"/>
+      <c r="S153" s="14"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A154" s="13"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5"/>
+      <c r="H154" s="5"/>
+      <c r="I154" s="5"/>
+      <c r="J154" s="5"/>
+      <c r="K154" s="5"/>
+      <c r="L154" s="5"/>
+      <c r="M154" s="5"/>
+      <c r="N154" s="5"/>
+      <c r="O154" s="5"/>
+      <c r="P154" s="5"/>
+      <c r="Q154" s="5"/>
+      <c r="R154" s="6"/>
+      <c r="S154" s="14"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A155" s="13"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="8"/>
+      <c r="F155" s="8"/>
+      <c r="G155" s="8"/>
+      <c r="H155" s="8"/>
+      <c r="I155" s="8"/>
+      <c r="J155" s="8"/>
+      <c r="K155" s="8"/>
+      <c r="L155" s="8"/>
+      <c r="M155" s="8"/>
+      <c r="N155" s="8"/>
+      <c r="O155" s="8"/>
+      <c r="P155" s="8"/>
+      <c r="Q155" s="8"/>
+      <c r="R155" s="9"/>
+      <c r="S155" s="14"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A156" s="13"/>
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="5"/>
+      <c r="I156" s="5"/>
+      <c r="J156" s="5"/>
+      <c r="K156" s="5"/>
+      <c r="L156" s="5"/>
+      <c r="M156" s="5"/>
+      <c r="N156" s="5"/>
+      <c r="O156" s="5"/>
+      <c r="P156" s="5"/>
+      <c r="Q156" s="5"/>
+      <c r="R156" s="5"/>
+      <c r="S156" s="14"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A157" s="13"/>
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+      <c r="G157" s="5"/>
+      <c r="H157" s="5"/>
+      <c r="I157" s="5"/>
+      <c r="J157" s="5"/>
+      <c r="K157" s="5"/>
+      <c r="L157" s="5"/>
+      <c r="M157" s="5"/>
+      <c r="N157" s="5"/>
+      <c r="O157" s="5"/>
+      <c r="P157" s="5"/>
+      <c r="Q157" s="5"/>
+      <c r="R157" s="5"/>
+      <c r="S157" s="14"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A158" s="13"/>
+      <c r="B158" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
+      <c r="J158" s="2"/>
+      <c r="K158" s="2"/>
+      <c r="L158" s="2"/>
+      <c r="M158" s="2"/>
+      <c r="N158" s="2"/>
+      <c r="O158" s="2"/>
+      <c r="P158" s="2"/>
+      <c r="Q158" s="2"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="14"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A159" s="13"/>
+      <c r="B159" s="4"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+      <c r="G159" s="5"/>
+      <c r="H159" s="5"/>
+      <c r="I159" s="5"/>
+      <c r="J159" s="5"/>
+      <c r="K159" s="5"/>
+      <c r="L159" s="5"/>
+      <c r="M159" s="5"/>
+      <c r="N159" s="5"/>
+      <c r="O159" s="5"/>
+      <c r="P159" s="5"/>
+      <c r="Q159" s="5"/>
+      <c r="R159" s="6"/>
+      <c r="S159" s="14"/>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A160" s="13"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+      <c r="G160" s="5"/>
+      <c r="H160" s="5"/>
+      <c r="I160" s="5"/>
+      <c r="J160" s="5"/>
+      <c r="K160" s="5"/>
+      <c r="L160" s="5"/>
+      <c r="M160" s="5"/>
+      <c r="N160" s="5"/>
+      <c r="O160" s="5"/>
+      <c r="P160" s="5"/>
+      <c r="Q160" s="5"/>
+      <c r="R160" s="6"/>
+      <c r="S160" s="14"/>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A161" s="13"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+      <c r="G161" s="5"/>
+      <c r="H161" s="5"/>
+      <c r="I161" s="5"/>
+      <c r="J161" s="5"/>
+      <c r="K161" s="5"/>
+      <c r="L161" s="5"/>
+      <c r="M161" s="5"/>
+      <c r="N161" s="5"/>
+      <c r="O161" s="5"/>
+      <c r="P161" s="5"/>
+      <c r="Q161" s="5"/>
+      <c r="R161" s="6"/>
+      <c r="S161" s="14"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A162" s="13"/>
+      <c r="B162" s="4"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+      <c r="G162" s="5"/>
+      <c r="H162" s="5"/>
+      <c r="I162" s="5"/>
+      <c r="J162" s="5"/>
+      <c r="K162" s="5"/>
+      <c r="L162" s="5"/>
+      <c r="M162" s="5"/>
+      <c r="N162" s="5"/>
+      <c r="O162" s="5"/>
+      <c r="P162" s="5"/>
+      <c r="Q162" s="5"/>
+      <c r="R162" s="6"/>
+      <c r="S162" s="14"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A163" s="13"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="5"/>
+      <c r="G163" s="5"/>
+      <c r="H163" s="5"/>
+      <c r="I163" s="5"/>
+      <c r="J163" s="5"/>
+      <c r="K163" s="5"/>
+      <c r="L163" s="5"/>
+      <c r="M163" s="5"/>
+      <c r="N163" s="5"/>
+      <c r="O163" s="5"/>
+      <c r="P163" s="5"/>
+      <c r="Q163" s="5"/>
+      <c r="R163" s="6"/>
+      <c r="S163" s="14"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A164" s="13"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
+      <c r="G164" s="5"/>
+      <c r="H164" s="5"/>
+      <c r="I164" s="5"/>
+      <c r="J164" s="5"/>
+      <c r="K164" s="5"/>
+      <c r="L164" s="5"/>
+      <c r="M164" s="5"/>
+      <c r="N164" s="5"/>
+      <c r="O164" s="5"/>
+      <c r="P164" s="5"/>
+      <c r="Q164" s="5"/>
+      <c r="R164" s="6"/>
+      <c r="S164" s="14"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A165" s="13"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="5"/>
+      <c r="G165" s="5"/>
+      <c r="H165" s="5"/>
+      <c r="I165" s="5"/>
+      <c r="J165" s="5"/>
+      <c r="K165" s="5"/>
+      <c r="L165" s="5"/>
+      <c r="M165" s="5"/>
+      <c r="N165" s="5"/>
+      <c r="O165" s="5"/>
+      <c r="P165" s="5"/>
+      <c r="Q165" s="5"/>
+      <c r="R165" s="6"/>
+      <c r="S165" s="14"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A166" s="13"/>
+      <c r="B166" s="4"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+      <c r="G166" s="5"/>
+      <c r="H166" s="5"/>
+      <c r="I166" s="5"/>
+      <c r="J166" s="5"/>
+      <c r="K166" s="5"/>
+      <c r="L166" s="5"/>
+      <c r="M166" s="5"/>
+      <c r="N166" s="5"/>
+      <c r="O166" s="5"/>
+      <c r="P166" s="5"/>
+      <c r="Q166" s="5"/>
+      <c r="R166" s="6"/>
+      <c r="S166" s="14"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A167" s="13"/>
+      <c r="B167" s="4"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="5"/>
+      <c r="G167" s="5"/>
+      <c r="H167" s="5"/>
+      <c r="I167" s="5"/>
+      <c r="J167" s="5"/>
+      <c r="K167" s="5"/>
+      <c r="L167" s="5"/>
+      <c r="M167" s="5"/>
+      <c r="N167" s="5"/>
+      <c r="O167" s="5"/>
+      <c r="P167" s="5"/>
+      <c r="Q167" s="5"/>
+      <c r="R167" s="6"/>
+      <c r="S167" s="14"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A168" s="13"/>
+      <c r="B168" s="4"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="5"/>
+      <c r="H168" s="5"/>
+      <c r="I168" s="5"/>
+      <c r="J168" s="5"/>
+      <c r="K168" s="5"/>
+      <c r="L168" s="5"/>
+      <c r="M168" s="5"/>
+      <c r="N168" s="5"/>
+      <c r="O168" s="5"/>
+      <c r="P168" s="5"/>
+      <c r="Q168" s="5"/>
+      <c r="R168" s="6"/>
+      <c r="S168" s="14"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A169" s="13"/>
+      <c r="B169" s="4"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="5"/>
+      <c r="G169" s="5"/>
+      <c r="H169" s="5"/>
+      <c r="I169" s="5"/>
+      <c r="J169" s="5"/>
+      <c r="K169" s="5"/>
+      <c r="L169" s="5"/>
+      <c r="M169" s="5"/>
+      <c r="N169" s="5"/>
+      <c r="O169" s="5"/>
+      <c r="P169" s="5"/>
+      <c r="Q169" s="5"/>
+      <c r="R169" s="6"/>
+      <c r="S169" s="14"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A170" s="13"/>
+      <c r="B170" s="4"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+      <c r="G170" s="5"/>
+      <c r="H170" s="5"/>
+      <c r="I170" s="5"/>
+      <c r="J170" s="5"/>
+      <c r="K170" s="5"/>
+      <c r="L170" s="5"/>
+      <c r="M170" s="5"/>
+      <c r="N170" s="5"/>
+      <c r="O170" s="5"/>
+      <c r="P170" s="5"/>
+      <c r="Q170" s="5"/>
+      <c r="R170" s="6"/>
+      <c r="S170" s="14"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A171" s="13"/>
+      <c r="B171" s="4"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+      <c r="G171" s="5"/>
+      <c r="H171" s="5"/>
+      <c r="I171" s="5"/>
+      <c r="J171" s="5"/>
+      <c r="K171" s="5"/>
+      <c r="L171" s="5"/>
+      <c r="M171" s="5"/>
+      <c r="N171" s="5"/>
+      <c r="O171" s="5"/>
+      <c r="P171" s="5"/>
+      <c r="Q171" s="5"/>
+      <c r="R171" s="6"/>
+      <c r="S171" s="14"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A172" s="13"/>
+      <c r="B172" s="4"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="5"/>
+      <c r="H172" s="5"/>
+      <c r="I172" s="5"/>
+      <c r="J172" s="5"/>
+      <c r="K172" s="5"/>
+      <c r="L172" s="5"/>
+      <c r="M172" s="5"/>
+      <c r="N172" s="5"/>
+      <c r="O172" s="5"/>
+      <c r="P172" s="5"/>
+      <c r="Q172" s="5"/>
+      <c r="R172" s="6"/>
+      <c r="S172" s="14"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A173" s="13"/>
+      <c r="B173" s="4"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="5"/>
+      <c r="G173" s="5"/>
+      <c r="H173" s="5"/>
+      <c r="I173" s="5"/>
+      <c r="J173" s="5"/>
+      <c r="K173" s="5"/>
+      <c r="L173" s="5"/>
+      <c r="M173" s="5"/>
+      <c r="N173" s="5"/>
+      <c r="O173" s="5"/>
+      <c r="P173" s="5"/>
+      <c r="Q173" s="5"/>
+      <c r="R173" s="6"/>
+      <c r="S173" s="14"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A174" s="13"/>
+      <c r="B174" s="4"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+      <c r="G174" s="5"/>
+      <c r="H174" s="5"/>
+      <c r="I174" s="5"/>
+      <c r="J174" s="5"/>
+      <c r="K174" s="5"/>
+      <c r="L174" s="5"/>
+      <c r="M174" s="5"/>
+      <c r="N174" s="5"/>
+      <c r="O174" s="5"/>
+      <c r="P174" s="5"/>
+      <c r="Q174" s="5"/>
+      <c r="R174" s="6"/>
+      <c r="S174" s="14"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A175" s="13"/>
+      <c r="B175" s="4"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="5"/>
+      <c r="G175" s="5"/>
+      <c r="H175" s="5"/>
+      <c r="I175" s="5"/>
+      <c r="J175" s="5"/>
+      <c r="K175" s="5"/>
+      <c r="L175" s="5"/>
+      <c r="M175" s="5"/>
+      <c r="N175" s="5"/>
+      <c r="O175" s="5"/>
+      <c r="P175" s="5"/>
+      <c r="Q175" s="5"/>
+      <c r="R175" s="6"/>
+      <c r="S175" s="14"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A176" s="13"/>
+      <c r="B176" s="4"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="5"/>
+      <c r="G176" s="5"/>
+      <c r="H176" s="5"/>
+      <c r="I176" s="5"/>
+      <c r="J176" s="5"/>
+      <c r="K176" s="5"/>
+      <c r="L176" s="5"/>
+      <c r="M176" s="5"/>
+      <c r="N176" s="5"/>
+      <c r="O176" s="5"/>
+      <c r="P176" s="5"/>
+      <c r="Q176" s="5"/>
+      <c r="R176" s="6"/>
+      <c r="S176" s="14"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A177" s="13"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+      <c r="G177" s="5"/>
+      <c r="H177" s="5"/>
+      <c r="I177" s="5"/>
+      <c r="J177" s="5"/>
+      <c r="K177" s="5"/>
+      <c r="L177" s="5"/>
+      <c r="M177" s="5"/>
+      <c r="N177" s="5"/>
+      <c r="O177" s="5"/>
+      <c r="P177" s="5"/>
+      <c r="Q177" s="5"/>
+      <c r="R177" s="6"/>
+      <c r="S177" s="14"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A178" s="13"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="5"/>
+      <c r="H178" s="5"/>
+      <c r="I178" s="5"/>
+      <c r="J178" s="5"/>
+      <c r="K178" s="5"/>
+      <c r="L178" s="5"/>
+      <c r="M178" s="5"/>
+      <c r="N178" s="5"/>
+      <c r="O178" s="5"/>
+      <c r="P178" s="5"/>
+      <c r="Q178" s="5"/>
+      <c r="R178" s="6"/>
+      <c r="S178" s="14"/>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A179" s="13"/>
+      <c r="B179" s="4"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="5"/>
+      <c r="H179" s="5"/>
+      <c r="I179" s="5"/>
+      <c r="J179" s="5"/>
+      <c r="K179" s="5"/>
+      <c r="L179" s="5"/>
+      <c r="M179" s="5"/>
+      <c r="N179" s="5"/>
+      <c r="O179" s="5"/>
+      <c r="P179" s="5"/>
+      <c r="Q179" s="5"/>
+      <c r="R179" s="6"/>
+      <c r="S179" s="14"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A180" s="13"/>
+      <c r="B180" s="4"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="5"/>
+      <c r="I180" s="5"/>
+      <c r="J180" s="5"/>
+      <c r="K180" s="5"/>
+      <c r="L180" s="5"/>
+      <c r="M180" s="5"/>
+      <c r="N180" s="5"/>
+      <c r="O180" s="5"/>
+      <c r="P180" s="5"/>
+      <c r="Q180" s="5"/>
+      <c r="R180" s="6"/>
+      <c r="S180" s="14"/>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A181" s="13"/>
+      <c r="B181" s="4"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="5"/>
+      <c r="H181" s="5"/>
+      <c r="I181" s="5"/>
+      <c r="J181" s="5"/>
+      <c r="K181" s="5"/>
+      <c r="L181" s="5"/>
+      <c r="M181" s="5"/>
+      <c r="N181" s="5"/>
+      <c r="O181" s="5"/>
+      <c r="P181" s="5"/>
+      <c r="Q181" s="5"/>
+      <c r="R181" s="6"/>
+      <c r="S181" s="14"/>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A182" s="13"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="8"/>
+      <c r="D182" s="8"/>
+      <c r="E182" s="8"/>
+      <c r="F182" s="8"/>
+      <c r="G182" s="8"/>
+      <c r="H182" s="8"/>
+      <c r="I182" s="8"/>
+      <c r="J182" s="8"/>
+      <c r="K182" s="8"/>
+      <c r="L182" s="8"/>
+      <c r="M182" s="8"/>
+      <c r="N182" s="8"/>
+      <c r="O182" s="8"/>
+      <c r="P182" s="8"/>
+      <c r="Q182" s="8"/>
+      <c r="R182" s="9"/>
+      <c r="S182" s="14"/>
+    </row>
+    <row r="183" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="15"/>
+      <c r="B183" s="16"/>
+      <c r="C183" s="16"/>
+      <c r="D183" s="16"/>
+      <c r="E183" s="16"/>
+      <c r="F183" s="16"/>
+      <c r="G183" s="16"/>
+      <c r="H183" s="16"/>
+      <c r="I183" s="16"/>
+      <c r="J183" s="16"/>
+      <c r="K183" s="16"/>
+      <c r="L183" s="16"/>
+      <c r="M183" s="16"/>
+      <c r="N183" s="16"/>
+      <c r="O183" s="16"/>
+      <c r="P183" s="16"/>
+      <c r="Q183" s="16"/>
+      <c r="R183" s="16"/>
+      <c r="S183" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Generate an encoded access token containing the user details
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/5.authentication-using-access-tokens.xlsx
+++ b/me/4.create-a-restful-api/5.authentication-using-access-tokens.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD327A38-516D-4CCF-92DF-FAD513142A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4422277A-7522-48D8-8DB2-4C9F43C010E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="introduction" sheetId="1" r:id="rId1"/>
     <sheet name="login endpoint and 400 status" sheetId="2" r:id="rId2"/>
     <sheet name="Select the user record" sheetId="3" r:id="rId3"/>
     <sheet name="Check username and pwd 401 code" sheetId="4" r:id="rId4"/>
+    <sheet name="Generate encoded access token" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="144">
   <si>
     <t>An introduction to authentication using access tokens</t>
   </si>
@@ -439,6 +440,60 @@
   <si>
     <t>call api /login.php với thông tin login request là username và password với thông tin username đúng  -&gt;  status code là 200</t>
   </si>
+  <si>
+    <t>Generate an encoded access token containing the user details</t>
+  </si>
+  <si>
+    <t>$payload = [</t>
+  </si>
+  <si>
+    <t>    "id" =&gt; $user["id"],</t>
+  </si>
+  <si>
+    <t>    "name" =&gt; $user["name"]</t>
+  </si>
+  <si>
+    <t>];</t>
+  </si>
+  <si>
+    <t>$access_token = base64_encode(json_encode($payload));</t>
+  </si>
+  <si>
+    <t>echo json_encode([</t>
+  </si>
+  <si>
+    <t>    "access_token" =&gt; $access_token</t>
+  </si>
+  <si>
+    <t>]);</t>
+  </si>
+  <si>
+    <t>Sau khi authenticatin thông tin login xong mình sẽ dùng thông tin login sau khi authentication xong tạo ra chuỗi access token dùng để authentication cho api mà ko cần thực hiện truy vấn</t>
+  </si>
+  <si>
+    <t>đến DB(giống như api key) để authentication mỗi khi có request đến api</t>
+  </si>
+  <si>
+    <t>Mình sẽ dùng id và name của user đã login đó để tạo ra access token, access token cũng giống như api key nó là 1 chuỗi được request đi trong header giống như api key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Để mình họa thì mình sẽ dùng hàm mã hóa base64_encode(). base64_encode() thường dùng để mã hóa sang các ký tự ASCII để gửi qua email hay url và được dùng kết hợp với base64_decode() </t>
+  </si>
+  <si>
+    <t>json_encode() để được 1 chuỗi rồi dùng chuỗi đó mã hóa thành access token bằng base64_encode()</t>
+  </si>
+  <si>
+    <t>base64_encode</t>
+  </si>
+  <si>
+    <t>https://www.php.net/manual/en/function.base64-encode.php</t>
+  </si>
+  <si>
+    <t>để decode các ký tự mã hóa đó về chuỗi ban đầu</t>
+  </si>
+  <si>
+    <t>call /login.php api</t>
+  </si>
 </sst>
 </file>
 
@@ -646,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -677,6 +732,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3344,6 +3401,205 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>127438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AD15768-005D-E899-44E4-F2B4D9A3A3D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="2009775"/>
+          <a:ext cx="11315700" cy="4785163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{574B622F-2E18-246C-3D7E-04020E590856}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="3381375"/>
+          <a:ext cx="19050" cy="21869400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>417848</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>18501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2E3102-3A27-EF57-6C7D-226E3FA6A532}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="26870025"/>
+          <a:ext cx="10019048" cy="4390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E720E7A1-C219-444D-A425-6C2F7876AA02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2152650" y="25879425"/>
+          <a:ext cx="533400" cy="4895850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12569,8 +12825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9DD791-CAFA-459E-BB7B-B2DEB3048E8F}">
   <dimension ref="A2:S198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="L94" sqref="L94"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15834,4 +16090,2375 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055F4B0F-C6EE-49FA-94E8-152DEDCB144F}">
+  <dimension ref="A2:T165"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="M136" sqref="M136"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="6"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="6"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="6"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="6"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="6"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="6"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="6"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="6"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="6"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="6"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="6"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="9"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="B41" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="22"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="24"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="24"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="24"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="24"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="24"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="24"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="24"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="24"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="24"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="24"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="24"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="19"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="24"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="24"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="19"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="24"/>
+      <c r="K55" t="s">
+        <v>47</v>
+      </c>
+      <c r="L55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="24"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="24"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="24"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="19"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="24"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="24"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="19"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="24"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="19"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="24"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="24"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="19"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="24"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="19"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="24"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="19"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="24"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="19"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="24"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="19"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="24"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="24"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="24"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="19"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="24"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="19"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="26"/>
+      <c r="I72" s="26"/>
+      <c r="J72" s="27"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="6"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="6"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="6"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="6"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="6"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="6"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="6"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="6"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="6"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="6"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="6"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="6"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="6"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="6"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="6"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="6"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="6"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="4"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="6"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="6"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="6"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="6"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="4"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="6"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="6"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="6"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="6"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="6"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="6"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="6"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="4"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="6"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="6"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="4"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="6"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="6"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+      <c r="I113" s="6"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="6"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="6"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="6"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="6"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="6"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="6"/>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="6"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="6"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+      <c r="I122" s="6"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
+      <c r="H123" s="5"/>
+      <c r="I123" s="6"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="5"/>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="5"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="5"/>
+      <c r="I127" s="6"/>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="5"/>
+      <c r="I128" s="6"/>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B129" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
+      <c r="H129" s="5"/>
+      <c r="I129" s="6"/>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B130" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="5"/>
+      <c r="I130" s="6"/>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B131" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="5"/>
+      <c r="I131" s="6"/>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B132" s="28"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="5"/>
+      <c r="I132" s="6"/>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B133" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5"/>
+      <c r="H133" s="5"/>
+      <c r="I133" s="6"/>
+      <c r="J133" t="s">
+        <v>47</v>
+      </c>
+      <c r="K133" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B134" s="28"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+      <c r="G134" s="5"/>
+      <c r="H134" s="5"/>
+      <c r="I134" s="6"/>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B135" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+      <c r="G135" s="5"/>
+      <c r="H135" s="5"/>
+      <c r="I135" s="6"/>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B136" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="5"/>
+      <c r="I136" s="6"/>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B137" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C137" s="8"/>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
+      <c r="F137" s="8"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
+      <c r="I137" s="9"/>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A140" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
+      <c r="O140" s="2"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
+      <c r="R140" s="3"/>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="5"/>
+      <c r="J141" s="5"/>
+      <c r="K141" s="5"/>
+      <c r="L141" s="5"/>
+      <c r="M141" s="5"/>
+      <c r="N141" s="5"/>
+      <c r="O141" s="5"/>
+      <c r="P141" s="5"/>
+      <c r="Q141" s="5"/>
+      <c r="R141" s="6"/>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="5"/>
+      <c r="J142" s="5"/>
+      <c r="K142" s="5"/>
+      <c r="L142" s="5"/>
+      <c r="M142" s="5"/>
+      <c r="N142" s="5"/>
+      <c r="O142" s="5"/>
+      <c r="P142" s="5"/>
+      <c r="Q142" s="5"/>
+      <c r="R142" s="6"/>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5"/>
+      <c r="H143" s="5"/>
+      <c r="I143" s="5"/>
+      <c r="J143" s="5"/>
+      <c r="K143" s="5"/>
+      <c r="L143" s="5"/>
+      <c r="M143" s="5"/>
+      <c r="N143" s="5"/>
+      <c r="O143" s="5"/>
+      <c r="P143" s="5"/>
+      <c r="Q143" s="5"/>
+      <c r="R143" s="6"/>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5"/>
+      <c r="H144" s="5"/>
+      <c r="I144" s="5"/>
+      <c r="J144" s="5"/>
+      <c r="K144" s="5"/>
+      <c r="L144" s="5"/>
+      <c r="M144" s="5"/>
+      <c r="N144" s="5"/>
+      <c r="O144" s="5"/>
+      <c r="P144" s="5"/>
+      <c r="Q144" s="5"/>
+      <c r="R144" s="6"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+      <c r="I145" s="5"/>
+      <c r="J145" s="5"/>
+      <c r="K145" s="5"/>
+      <c r="L145" s="5"/>
+      <c r="M145" s="5"/>
+      <c r="N145" s="5"/>
+      <c r="O145" s="5"/>
+      <c r="P145" s="5"/>
+      <c r="Q145" s="5"/>
+      <c r="R145" s="6"/>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A146" s="4"/>
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="J146" s="5"/>
+      <c r="K146" s="5"/>
+      <c r="L146" s="5"/>
+      <c r="M146" s="5"/>
+      <c r="N146" s="5"/>
+      <c r="O146" s="5"/>
+      <c r="P146" s="5"/>
+      <c r="Q146" s="5"/>
+      <c r="R146" s="6"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5"/>
+      <c r="H147" s="5"/>
+      <c r="I147" s="5"/>
+      <c r="J147" s="5"/>
+      <c r="K147" s="5"/>
+      <c r="L147" s="5"/>
+      <c r="M147" s="5"/>
+      <c r="N147" s="5"/>
+      <c r="O147" s="5"/>
+      <c r="P147" s="5"/>
+      <c r="Q147" s="5"/>
+      <c r="R147" s="6"/>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+      <c r="G148" s="5"/>
+      <c r="H148" s="5"/>
+      <c r="I148" s="5"/>
+      <c r="J148" s="5"/>
+      <c r="K148" s="5"/>
+      <c r="L148" s="5"/>
+      <c r="M148" s="5"/>
+      <c r="N148" s="5"/>
+      <c r="O148" s="5"/>
+      <c r="P148" s="5"/>
+      <c r="Q148" s="5"/>
+      <c r="R148" s="6"/>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5"/>
+      <c r="H149" s="5"/>
+      <c r="I149" s="5"/>
+      <c r="J149" s="5"/>
+      <c r="K149" s="5"/>
+      <c r="L149" s="5"/>
+      <c r="M149" s="5"/>
+      <c r="N149" s="5"/>
+      <c r="O149" s="5"/>
+      <c r="P149" s="5"/>
+      <c r="Q149" s="5"/>
+      <c r="R149" s="6"/>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="5"/>
+      <c r="I150" s="5"/>
+      <c r="J150" s="5"/>
+      <c r="K150" s="5"/>
+      <c r="L150" s="5"/>
+      <c r="M150" s="5"/>
+      <c r="N150" s="5"/>
+      <c r="O150" s="5"/>
+      <c r="P150" s="5"/>
+      <c r="Q150" s="5"/>
+      <c r="R150" s="6"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="5"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="5"/>
+      <c r="H151" s="5"/>
+      <c r="I151" s="5"/>
+      <c r="J151" s="5"/>
+      <c r="K151" s="5"/>
+      <c r="L151" s="5"/>
+      <c r="M151" s="5"/>
+      <c r="N151" s="5"/>
+      <c r="O151" s="5"/>
+      <c r="P151" s="5"/>
+      <c r="Q151" s="5"/>
+      <c r="R151" s="6"/>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="5"/>
+      <c r="I152" s="5"/>
+      <c r="J152" s="5"/>
+      <c r="K152" s="5"/>
+      <c r="L152" s="5"/>
+      <c r="M152" s="5"/>
+      <c r="N152" s="5"/>
+      <c r="O152" s="5"/>
+      <c r="P152" s="5"/>
+      <c r="Q152" s="5"/>
+      <c r="R152" s="6"/>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+      <c r="G153" s="5"/>
+      <c r="H153" s="5"/>
+      <c r="I153" s="5"/>
+      <c r="J153" s="5"/>
+      <c r="K153" s="5"/>
+      <c r="L153" s="5"/>
+      <c r="M153" s="5"/>
+      <c r="N153" s="5"/>
+      <c r="O153" s="5"/>
+      <c r="P153" s="5"/>
+      <c r="Q153" s="5"/>
+      <c r="R153" s="6"/>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5"/>
+      <c r="H154" s="5"/>
+      <c r="I154" s="5"/>
+      <c r="J154" s="5"/>
+      <c r="K154" s="5"/>
+      <c r="L154" s="5"/>
+      <c r="M154" s="5"/>
+      <c r="N154" s="5"/>
+      <c r="O154" s="5"/>
+      <c r="P154" s="5"/>
+      <c r="Q154" s="5"/>
+      <c r="R154" s="6"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+      <c r="G155" s="5"/>
+      <c r="H155" s="5"/>
+      <c r="I155" s="5"/>
+      <c r="J155" s="5"/>
+      <c r="K155" s="5"/>
+      <c r="L155" s="5"/>
+      <c r="M155" s="5"/>
+      <c r="N155" s="5"/>
+      <c r="O155" s="5"/>
+      <c r="P155" s="5"/>
+      <c r="Q155" s="5"/>
+      <c r="R155" s="6"/>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="5"/>
+      <c r="I156" s="5"/>
+      <c r="J156" s="5"/>
+      <c r="K156" s="5"/>
+      <c r="L156" s="5"/>
+      <c r="M156" s="5"/>
+      <c r="N156" s="5"/>
+      <c r="O156" s="5"/>
+      <c r="P156" s="5"/>
+      <c r="Q156" s="5"/>
+      <c r="R156" s="6"/>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+      <c r="G157" s="5"/>
+      <c r="H157" s="5"/>
+      <c r="I157" s="5"/>
+      <c r="J157" s="5"/>
+      <c r="K157" s="5"/>
+      <c r="L157" s="5"/>
+      <c r="M157" s="5"/>
+      <c r="N157" s="5"/>
+      <c r="O157" s="5"/>
+      <c r="P157" s="5"/>
+      <c r="Q157" s="5"/>
+      <c r="R157" s="6"/>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A158" s="4"/>
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="5"/>
+      <c r="F158" s="5"/>
+      <c r="G158" s="5"/>
+      <c r="H158" s="5"/>
+      <c r="I158" s="5"/>
+      <c r="J158" s="5"/>
+      <c r="K158" s="5"/>
+      <c r="L158" s="5"/>
+      <c r="M158" s="5"/>
+      <c r="N158" s="5"/>
+      <c r="O158" s="5"/>
+      <c r="P158" s="5"/>
+      <c r="Q158" s="5"/>
+      <c r="R158" s="6"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A159" s="4"/>
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+      <c r="G159" s="5"/>
+      <c r="H159" s="5"/>
+      <c r="I159" s="5"/>
+      <c r="J159" s="5"/>
+      <c r="K159" s="5"/>
+      <c r="L159" s="5"/>
+      <c r="M159" s="5"/>
+      <c r="N159" s="5"/>
+      <c r="O159" s="5"/>
+      <c r="P159" s="5"/>
+      <c r="Q159" s="5"/>
+      <c r="R159" s="6"/>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A160" s="4"/>
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+      <c r="G160" s="5"/>
+      <c r="H160" s="5"/>
+      <c r="I160" s="5"/>
+      <c r="J160" s="5"/>
+      <c r="K160" s="5"/>
+      <c r="L160" s="5"/>
+      <c r="M160" s="5"/>
+      <c r="N160" s="5"/>
+      <c r="O160" s="5"/>
+      <c r="P160" s="5"/>
+      <c r="Q160" s="5"/>
+      <c r="R160" s="6"/>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A161" s="4"/>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+      <c r="G161" s="5"/>
+      <c r="H161" s="5"/>
+      <c r="I161" s="5"/>
+      <c r="J161" s="5"/>
+      <c r="K161" s="5"/>
+      <c r="L161" s="5"/>
+      <c r="M161" s="5"/>
+      <c r="N161" s="5"/>
+      <c r="O161" s="5"/>
+      <c r="P161" s="5"/>
+      <c r="Q161" s="5"/>
+      <c r="R161" s="6"/>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A162" s="4"/>
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+      <c r="G162" s="5"/>
+      <c r="H162" s="5"/>
+      <c r="I162" s="5"/>
+      <c r="J162" s="5"/>
+      <c r="K162" s="5"/>
+      <c r="L162" s="5"/>
+      <c r="M162" s="5"/>
+      <c r="N162" s="5"/>
+      <c r="O162" s="5"/>
+      <c r="P162" s="5"/>
+      <c r="Q162" s="5"/>
+      <c r="R162" s="6"/>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A163" s="4"/>
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="5"/>
+      <c r="G163" s="5"/>
+      <c r="H163" s="5"/>
+      <c r="I163" s="5"/>
+      <c r="J163" s="5"/>
+      <c r="K163" s="5"/>
+      <c r="L163" s="5"/>
+      <c r="M163" s="5"/>
+      <c r="N163" s="5"/>
+      <c r="O163" s="5"/>
+      <c r="P163" s="5"/>
+      <c r="Q163" s="5"/>
+      <c r="R163" s="6"/>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A164" s="4"/>
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
+      <c r="G164" s="5"/>
+      <c r="H164" s="5"/>
+      <c r="I164" s="5"/>
+      <c r="J164" s="5"/>
+      <c r="K164" s="5"/>
+      <c r="L164" s="5"/>
+      <c r="M164" s="5"/>
+      <c r="N164" s="5"/>
+      <c r="O164" s="5"/>
+      <c r="P164" s="5"/>
+      <c r="Q164" s="5"/>
+      <c r="R164" s="6"/>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A165" s="7"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="8"/>
+      <c r="D165" s="8"/>
+      <c r="E165" s="8"/>
+      <c r="F165" s="8"/>
+      <c r="G165" s="8"/>
+      <c r="H165" s="8"/>
+      <c r="I165" s="8"/>
+      <c r="J165" s="8"/>
+      <c r="K165" s="8"/>
+      <c r="L165" s="8"/>
+      <c r="M165" s="8"/>
+      <c r="N165" s="8"/>
+      <c r="O165" s="8"/>
+      <c r="P165" s="8"/>
+      <c r="Q165" s="8"/>
+      <c r="R165" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>